<commit_message>
Revision on coil list for Htl building type
</commit_message>
<xml_diff>
--- a/commercial measures/SWHC027-08 Package Terminal ACHP/SWHC027-08 Package Terminal ACHP_Htl_Ex/coil_list.xlsx
+++ b/commercial measures/SWHC027-08 Package Terminal ACHP/SWHC027-08 Package Terminal ACHP_Htl_Ex/coil_list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEER Models\T24 Code Update\SWHC027-08\commercial measures\SWHC027-08 Package Terminal ACHP\SWHC027-08 Package Terminal ACHP_Htl_Ex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEER Models\T24 Code Update\SWHC027-08-coil-list\commercial measures\SWHC027-08 Package Terminal ACHP\SWHC027-08 Package Terminal ACHP_Htl_Ex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623055C0-7236-4E08-800F-DE2351842DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC404DEA-3C80-406A-9F95-DFF7957FF3C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="-16200" windowWidth="14610" windowHeight="15585" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
   <si>
     <t>coil type</t>
   </si>
@@ -78,42 +78,6 @@
   </si>
   <si>
     <t>OFFICE EL1 EAST PERIM SPC (G.E3) SZ-CAV COOLING COIL</t>
-  </si>
-  <si>
-    <t>GUESTRM EL4 NNE PERIM SPC (G.NNE3) SZ-CAV COOLING COIL</t>
-  </si>
-  <si>
-    <t>GUESTRM EL4 NNE PERIM SPC (M.NNE13) SZ-CAV COOLING COIL</t>
-  </si>
-  <si>
-    <t>GUESTRM EL4 NNE PERIM SPC (T.NNE23) SZ-CAV COOLING COIL</t>
-  </si>
-  <si>
-    <t>GUESTRM EL4 NORTH PERIM SPC (G.N1) SZ-CAV COOLING COIL</t>
-  </si>
-  <si>
-    <t>GUESTRM EL4 NORTH PERIM SPC (M.N11) SZ-CAV COOLING COIL</t>
-  </si>
-  <si>
-    <t>GUESTRM EL4 NORTH PERIM SPC (T.N21) SZ-CAV COOLING COIL</t>
-  </si>
-  <si>
-    <t>GUESTRM EL4 SOUTH PERIM SPC (G.S4) SZ-CAV COOLING COIL</t>
-  </si>
-  <si>
-    <t>GUESTRM EL4 SOUTH PERIM SPC (M.S14) SZ-CAV COOLING COIL</t>
-  </si>
-  <si>
-    <t>GUESTRM EL4 SOUTH PERIM SPC (T.S24) SZ-CAV COOLING COIL</t>
-  </si>
-  <si>
-    <t>GUESTRM EL4 SSW PERIM SPC (G.SSW2) SZ-CAV COOLING COIL</t>
-  </si>
-  <si>
-    <t>GUESTRM EL4 SSW PERIM SPC (M.SSW12) SZ-CAV COOLING COIL</t>
-  </si>
-  <si>
-    <t>GUESTRM EL4 SSW PERIM SPC (T.SSW22) SZ-CAV COOLING COIL</t>
   </si>
   <si>
     <t>Htl</t>
@@ -347,10 +311,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -376,7 +340,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -387,7 +351,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -398,7 +362,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -409,7 +373,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -420,7 +384,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -431,7 +395,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -442,7 +406,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -453,7 +417,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -464,7 +428,7 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
@@ -475,142 +439,10 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -620,17 +452,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="977ed3b4-dc53-4ccd-91b7-93b67a0eba97">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="63e8c1f7-1787-49b1-80e5-dcc3ae9ab6e9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100366A9EB7EB4E4F489A4515111482199D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="db4c11ca1524f4dab84562af922705c9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="977ed3b4-dc53-4ccd-91b7-93b67a0eba97" xmlns:ns3="63e8c1f7-1787-49b1-80e5-dcc3ae9ab6e9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49dcd01241987285feedf33fb68cd0eb" ns2:_="" ns3:_="">
     <xsd:import namespace="977ed3b4-dc53-4ccd-91b7-93b67a0eba97"/>
@@ -879,6 +700,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="977ed3b4-dc53-4ccd-91b7-93b67a0eba97">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="63e8c1f7-1787-49b1-80e5-dcc3ae9ab6e9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -889,17 +721,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C793356-EF07-413F-8D70-1A41F14956B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="977ed3b4-dc53-4ccd-91b7-93b67a0eba97"/>
-    <ds:schemaRef ds:uri="63e8c1f7-1787-49b1-80e5-dcc3ae9ab6e9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA256F47-F75B-465B-8D4D-7AE387585A91}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -918,6 +739,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C793356-EF07-413F-8D70-1A41F14956B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="977ed3b4-dc53-4ccd-91b7-93b67a0eba97"/>
+    <ds:schemaRef ds:uri="63e8c1f7-1787-49b1-80e5-dcc3ae9ab6e9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8C53DED-152A-4CF6-8ABB-344A65C2B74B}">
   <ds:schemaRefs>

</xml_diff>